<commit_message>
update excel template and readme
</commit_message>
<xml_diff>
--- a/Global_Seagrass_transect_rawData.xlsx
+++ b/Global_Seagrass_transect_rawData.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W106"/>
+  <dimension ref="A1:X106"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -433,25 +433,25 @@
         <v>Lon</v>
       </c>
       <c r="J1" t="str">
+        <v>Coordinate Method</v>
+      </c>
+      <c r="K1" t="str">
         <v>Time (HH:mm:ss)</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>Collection Mode</v>
       </c>
-      <c r="L1" t="str">
-        <v>depth (cm)</v>
-      </c>
       <c r="M1" t="str">
-        <v>depth (m)</v>
+        <v>Depth (cm)</v>
       </c>
       <c r="N1" t="str">
+        <v>Depth m)</v>
+      </c>
+      <c r="O1" t="str">
         <v>Camera Type</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>GPS Type</v>
-      </c>
-      <c r="P1" t="str">
-        <v>Species %</v>
       </c>
       <c r="Q1" t="str">
         <v>Species %</v>
@@ -474,10 +474,13 @@
       <c r="W1" t="str">
         <v>Species %</v>
       </c>
+      <c r="X1" t="str">
+        <v>Species %</v>
+      </c>
     </row>
     <row r="2">
       <c r="F2" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G2" t="str">
         <v>HA02</v>
@@ -485,7 +488,7 @@
     </row>
     <row r="3">
       <c r="F3" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G3" t="str">
         <v>HA07</v>
@@ -493,7 +496,7 @@
     </row>
     <row r="4">
       <c r="F4" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G4" t="str">
         <v>HA08</v>
@@ -501,7 +504,7 @@
     </row>
     <row r="5">
       <c r="F5" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G5" t="str">
         <v>HA16</v>
@@ -509,7 +512,7 @@
     </row>
     <row r="6">
       <c r="F6" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G6" t="str">
         <v>HA18</v>
@@ -517,7 +520,7 @@
     </row>
     <row r="7">
       <c r="F7" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G7" t="str">
         <v>HA25</v>
@@ -525,7 +528,7 @@
     </row>
     <row r="8">
       <c r="F8" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G8" t="str">
         <v>HA26</v>
@@ -533,7 +536,7 @@
     </row>
     <row r="9">
       <c r="F9" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G9" t="str">
         <v>HA33</v>
@@ -541,7 +544,7 @@
     </row>
     <row r="10">
       <c r="F10" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G10" t="str">
         <v>HA38</v>
@@ -549,7 +552,7 @@
     </row>
     <row r="11">
       <c r="F11" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G11" t="str">
         <v>HA40</v>
@@ -557,7 +560,7 @@
     </row>
     <row r="12">
       <c r="F12" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G12" t="str">
         <v>HA44</v>
@@ -565,7 +568,7 @@
     </row>
     <row r="13">
       <c r="F13" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G13" t="str">
         <v>HA46</v>
@@ -573,7 +576,7 @@
     </row>
     <row r="14">
       <c r="F14" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G14" t="str">
         <v>HB09</v>
@@ -581,7 +584,7 @@
     </row>
     <row r="15">
       <c r="F15" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G15" t="str">
         <v>HB10</v>
@@ -589,7 +592,7 @@
     </row>
     <row r="16">
       <c r="F16" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G16" t="str">
         <v>HB15</v>
@@ -597,7 +600,7 @@
     </row>
     <row r="17">
       <c r="F17" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G17" t="str">
         <v>HB17</v>
@@ -605,7 +608,7 @@
     </row>
     <row r="18">
       <c r="F18" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G18" t="str">
         <v>HB22</v>
@@ -613,7 +616,7 @@
     </row>
     <row r="19">
       <c r="F19" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G19" t="str">
         <v>HB25</v>
@@ -621,7 +624,7 @@
     </row>
     <row r="20">
       <c r="F20" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G20" t="str">
         <v>HB28</v>
@@ -629,7 +632,7 @@
     </row>
     <row r="21">
       <c r="F21" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G21" t="str">
         <v>HB31</v>
@@ -637,7 +640,7 @@
     </row>
     <row r="22">
       <c r="F22" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G22" t="str">
         <v>HB35</v>
@@ -645,7 +648,7 @@
     </row>
     <row r="23">
       <c r="F23" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G23" t="str">
         <v>HB37</v>
@@ -653,7 +656,7 @@
     </row>
     <row r="24">
       <c r="F24" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G24" t="str">
         <v>HB39</v>
@@ -661,7 +664,7 @@
     </row>
     <row r="25">
       <c r="F25" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G25" t="str">
         <v>HB45</v>
@@ -669,7 +672,7 @@
     </row>
     <row r="26">
       <c r="F26" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G26" t="str">
         <v>HC05</v>
@@ -677,7 +680,7 @@
     </row>
     <row r="27">
       <c r="F27" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G27" t="str">
         <v>HC07</v>
@@ -685,7 +688,7 @@
     </row>
     <row r="28">
       <c r="F28" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G28" t="str">
         <v>HC10</v>
@@ -693,7 +696,7 @@
     </row>
     <row r="29">
       <c r="F29" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G29" t="str">
         <v>HC18</v>
@@ -701,7 +704,7 @@
     </row>
     <row r="30">
       <c r="F30" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G30" t="str">
         <v>HC19</v>
@@ -709,7 +712,7 @@
     </row>
     <row r="31">
       <c r="F31" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G31" t="str">
         <v>HC22</v>
@@ -717,7 +720,7 @@
     </row>
     <row r="32">
       <c r="F32" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G32" t="str">
         <v>HC26</v>
@@ -725,7 +728,7 @@
     </row>
     <row r="33">
       <c r="F33" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G33" t="str">
         <v>HC34</v>
@@ -733,7 +736,7 @@
     </row>
     <row r="34">
       <c r="F34" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G34" t="str">
         <v>HC35</v>
@@ -741,7 +744,7 @@
     </row>
     <row r="35">
       <c r="F35" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G35" t="str">
         <v>HC38</v>
@@ -749,7 +752,7 @@
     </row>
     <row r="36">
       <c r="F36" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G36" t="str">
         <v>HC43</v>
@@ -757,7 +760,7 @@
     </row>
     <row r="37">
       <c r="F37" t="str">
-        <v>Horizontal</v>
+        <v>Parallel</v>
       </c>
       <c r="G37" t="str">
         <v>HC44</v>
@@ -765,7 +768,7 @@
     </row>
     <row r="38">
       <c r="F38" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G38" t="str">
         <v>VA00</v>
@@ -773,7 +776,7 @@
     </row>
     <row r="39">
       <c r="F39" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G39" t="str">
         <v>VA05</v>
@@ -781,7 +784,7 @@
     </row>
     <row r="40">
       <c r="F40" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G40" t="str">
         <v>VA10</v>
@@ -789,7 +792,7 @@
     </row>
     <row r="41">
       <c r="F41" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G41" t="str">
         <v>VA15</v>
@@ -797,7 +800,7 @@
     </row>
     <row r="42">
       <c r="F42" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G42" t="str">
         <v>VA20</v>
@@ -805,7 +808,7 @@
     </row>
     <row r="43">
       <c r="F43" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G43" t="str">
         <v>VA25</v>
@@ -813,7 +816,7 @@
     </row>
     <row r="44">
       <c r="F44" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G44" t="str">
         <v>VA30</v>
@@ -821,7 +824,7 @@
     </row>
     <row r="45">
       <c r="F45" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G45" t="str">
         <v>VA35</v>
@@ -829,7 +832,7 @@
     </row>
     <row r="46">
       <c r="F46" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G46" t="str">
         <v>VA40</v>
@@ -837,7 +840,7 @@
     </row>
     <row r="47">
       <c r="F47" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G47" t="str">
         <v>VA45</v>
@@ -845,7 +848,7 @@
     </row>
     <row r="48">
       <c r="F48" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G48" t="str">
         <v>VA50</v>
@@ -853,7 +856,7 @@
     </row>
     <row r="49">
       <c r="F49" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G49" t="str">
         <v>VB00</v>
@@ -861,7 +864,7 @@
     </row>
     <row r="50">
       <c r="F50" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G50" t="str">
         <v>VB05</v>
@@ -869,7 +872,7 @@
     </row>
     <row r="51">
       <c r="F51" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G51" t="str">
         <v>VB10</v>
@@ -877,7 +880,7 @@
     </row>
     <row r="52">
       <c r="F52" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G52" t="str">
         <v>VB15</v>
@@ -885,7 +888,7 @@
     </row>
     <row r="53">
       <c r="F53" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G53" t="str">
         <v>VB20</v>
@@ -893,7 +896,7 @@
     </row>
     <row r="54">
       <c r="F54" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G54" t="str">
         <v>VB25</v>
@@ -901,7 +904,7 @@
     </row>
     <row r="55">
       <c r="F55" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G55" t="str">
         <v>VB30</v>
@@ -909,7 +912,7 @@
     </row>
     <row r="56">
       <c r="F56" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G56" t="str">
         <v>VB35</v>
@@ -917,7 +920,7 @@
     </row>
     <row r="57">
       <c r="F57" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G57" t="str">
         <v>VB40</v>
@@ -925,7 +928,7 @@
     </row>
     <row r="58">
       <c r="F58" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G58" t="str">
         <v>VB45</v>
@@ -933,7 +936,7 @@
     </row>
     <row r="59">
       <c r="F59" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G59" t="str">
         <v>VB50</v>
@@ -941,7 +944,7 @@
     </row>
     <row r="60">
       <c r="F60" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G60" t="str">
         <v>VC00</v>
@@ -949,7 +952,7 @@
     </row>
     <row r="61">
       <c r="F61" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G61" t="str">
         <v>VC05</v>
@@ -957,7 +960,7 @@
     </row>
     <row r="62">
       <c r="F62" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G62" t="str">
         <v>VC10</v>
@@ -965,7 +968,7 @@
     </row>
     <row r="63">
       <c r="F63" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G63" t="str">
         <v>VC15</v>
@@ -973,7 +976,7 @@
     </row>
     <row r="64">
       <c r="F64" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G64" t="str">
         <v>VC20</v>
@@ -981,7 +984,7 @@
     </row>
     <row r="65">
       <c r="F65" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G65" t="str">
         <v>VC25</v>
@@ -989,7 +992,7 @@
     </row>
     <row r="66">
       <c r="F66" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G66" t="str">
         <v>VC30</v>
@@ -997,7 +1000,7 @@
     </row>
     <row r="67">
       <c r="F67" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G67" t="str">
         <v>VC35</v>
@@ -1005,7 +1008,7 @@
     </row>
     <row r="68">
       <c r="F68" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G68" t="str">
         <v>VC40</v>
@@ -1013,7 +1016,7 @@
     </row>
     <row r="69">
       <c r="F69" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G69" t="str">
         <v>VC45</v>
@@ -1021,7 +1024,7 @@
     </row>
     <row r="70">
       <c r="F70" t="str">
-        <v>Vertical</v>
+        <v>Perpendicular</v>
       </c>
       <c r="G70" t="str">
         <v>VC50</v>
@@ -1032,7 +1035,7 @@
         <v>Random</v>
       </c>
       <c r="G71" t="str">
-        <v>R1</v>
+        <v>R01</v>
       </c>
     </row>
     <row r="72">
@@ -1040,7 +1043,7 @@
         <v>Random</v>
       </c>
       <c r="G72" t="str">
-        <v>R2</v>
+        <v>R02</v>
       </c>
     </row>
     <row r="73">
@@ -1048,7 +1051,7 @@
         <v>Random</v>
       </c>
       <c r="G73" t="str">
-        <v>R3</v>
+        <v>R03</v>
       </c>
     </row>
     <row r="74">
@@ -1056,7 +1059,7 @@
         <v>Random</v>
       </c>
       <c r="G74" t="str">
-        <v>R4</v>
+        <v>R04</v>
       </c>
     </row>
     <row r="75">
@@ -1064,7 +1067,7 @@
         <v>Random</v>
       </c>
       <c r="G75" t="str">
-        <v>R5</v>
+        <v>R05</v>
       </c>
     </row>
     <row r="76">
@@ -1072,7 +1075,7 @@
         <v>Random</v>
       </c>
       <c r="G76" t="str">
-        <v>R6</v>
+        <v>R06</v>
       </c>
     </row>
     <row r="77">
@@ -1080,7 +1083,7 @@
         <v>Random</v>
       </c>
       <c r="G77" t="str">
-        <v>R7</v>
+        <v>R07</v>
       </c>
     </row>
     <row r="78">
@@ -1088,7 +1091,7 @@
         <v>Random</v>
       </c>
       <c r="G78" t="str">
-        <v>R8</v>
+        <v>R08</v>
       </c>
     </row>
     <row r="79">
@@ -1096,7 +1099,7 @@
         <v>Random</v>
       </c>
       <c r="G79" t="str">
-        <v>R9</v>
+        <v>R09</v>
       </c>
     </row>
     <row r="80">
@@ -1317,7 +1320,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:W106"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:X106"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1496,7 +1499,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AA18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1516,12 +1519,6 @@
       <c r="B2" t="str">
         <v>Date the observation was recorded</v>
       </c>
-      <c r="U2" t="str">
-        <v>Species %</v>
-      </c>
-      <c r="V2" t="str">
-        <v>Species %</v>
-      </c>
       <c r="W2" t="str">
         <v/>
       </c>
@@ -1583,7 +1580,7 @@
         <v>Quadrat</v>
       </c>
       <c r="B8" t="str">
-        <v>The quadrat ID, constructed using the combination of transect type, row, column, and number according to the protocol description</v>
+        <v>The quadrat ID, constructed using the combination of transect type, row, column, and number of metres, according to the protocol description</v>
       </c>
     </row>
     <row r="9">
@@ -1604,63 +1601,71 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Time (HH:mm:ss)</v>
+        <v>Coordinate method</v>
       </c>
       <c r="B11" t="str">
-        <v>The time the observation was made in HH:mm:ss (ss optional)</v>
+        <v>Indicate whether the coordinate was obtained in the field with the GPS, or after field collection from the photo. One of "GPS" or "photo"</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>Collection Mode</v>
+        <v>Time (HH:mm:ss)</v>
       </c>
       <c r="B12" t="str">
-        <v>The mode of collection, e.g. walking, snorkling, scuba</v>
+        <v>The time the observation was made in HH:mm:ss (ss optional)</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>depth (cm)</v>
+        <v>Collection Mode</v>
       </c>
       <c r="B13" t="str">
-        <v>The depth of the observation in cm. For no depth, please put 0</v>
+        <v>The mode of collection, e.g. walking, snorkling, scuba</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>depth (m)</v>
+        <v>depth (cm)</v>
       </c>
       <c r="B14" t="str">
-        <v>The depth of the observation in metres</v>
+        <v>The depth of the observation in cm. For no depth, please put 0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Camera Type</v>
+        <v>depth (m)</v>
       </c>
       <c r="B15" t="str">
-        <v>The make and model of the camera used</v>
+        <v>The depth of the observation in metres</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>GPS Type</v>
+        <v>Camera Type</v>
       </c>
       <c r="B16" t="str">
-        <v>The make and model of the GPS used</v>
+        <v>The make and model of the camera used</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
+        <v>GPS Type</v>
+      </c>
+      <c r="B17" t="str">
+        <v>The make and model of the GPS used</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
         <v>Species %</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B18" t="str">
         <v>The percent cover of the species observed. For each column please replace "Species" with the full Genus-Species of the species</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AA17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AA18"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>